<commit_message>
Updated simple cascade for testing of new additions during development
</commit_message>
<xml_diff>
--- a/data/cascade-simple.xlsx
+++ b/data/cascade-simple.xlsx
@@ -1,23 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/training/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
+    <workbookView xWindow="-6140" yWindow="-23540" windowWidth="34600" windowHeight="19160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
     <sheet name="Characteristics" sheetId="4" r:id="rId3"/>
     <sheet name="Parameters" sheetId="3" r:id="rId4"/>
+    <sheet name="Databook Sheet Names" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Code Label</t>
   </si>
@@ -118,45 +132,6 @@
     <t>Vaccination Rate</t>
   </si>
   <si>
-    <t>Infection Rate (Vaccinated)</t>
-  </si>
-  <si>
-    <t>LTBI Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>LTBI-TB Progression Rate (Untreated)</t>
-  </si>
-  <si>
-    <t>LTBI Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>LTBI-TB Progression Rate (Treated)</t>
-  </si>
-  <si>
-    <t>LTBI Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>TB Treatment Uptake Rate</t>
-  </si>
-  <si>
-    <t>TB Death Rate (Untreated)</t>
-  </si>
-  <si>
-    <t>TB Treatment Abandonment Rate</t>
-  </si>
-  <si>
-    <t>TB Treatment Success Rate</t>
-  </si>
-  <si>
-    <t>TB Death Rate (Treated)</t>
-  </si>
-  <si>
-    <t>Reinfection Rate (Recovered)</t>
-  </si>
-  <si>
-    <t>Infection Rate (Susceptible)</t>
-  </si>
-  <si>
     <t>v_rate</t>
   </si>
   <si>
@@ -166,39 +141,6 @@
     <t>infv_rate</t>
   </si>
   <si>
-    <t>ltyes_rate</t>
-  </si>
-  <si>
-    <t>ltno_rate</t>
-  </si>
-  <si>
-    <t>ltsuc_rate</t>
-  </si>
-  <si>
-    <t>ltup_rate</t>
-  </si>
-  <si>
-    <t>lttp_rate</t>
-  </si>
-  <si>
-    <t>acyes_rate</t>
-  </si>
-  <si>
-    <t>acno_rate</t>
-  </si>
-  <si>
-    <t>acud_rate</t>
-  </si>
-  <si>
-    <t>acsuc_rate</t>
-  </si>
-  <si>
-    <t>actd_rate</t>
-  </si>
-  <si>
-    <t>infr_rate</t>
-  </si>
-  <si>
     <t>Includes</t>
   </si>
   <si>
@@ -218,6 +160,162 @@
   </si>
   <si>
     <t>Transition Tag</t>
+  </si>
+  <si>
+    <t>Plot Coordinates</t>
+  </si>
+  <si>
+    <t>Dead Tag</t>
+  </si>
+  <si>
+    <t>No Plot</t>
+  </si>
+  <si>
+    <t>Databook Order</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Entry Point</t>
+  </si>
+  <si>
+    <t>Plot Percentage</t>
+  </si>
+  <si>
+    <t>alive</t>
+  </si>
+  <si>
+    <t>Active prevalence</t>
+  </si>
+  <si>
+    <t>lt_treat</t>
+  </si>
+  <si>
+    <t>Treated latent infect</t>
+  </si>
+  <si>
+    <t>Treated active infections</t>
+  </si>
+  <si>
+    <t>at_treat</t>
+  </si>
+  <si>
+    <t>Vacinated individuals</t>
+  </si>
+  <si>
+    <t>vaccin</t>
+  </si>
+  <si>
+    <t>Junction</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Sheet Label</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>sh_pop</t>
+  </si>
+  <si>
+    <t>Latent Infection Rate (Susceptible)</t>
+  </si>
+  <si>
+    <t>Latent Infection Rate (Vaccinated)</t>
+  </si>
+  <si>
+    <t>Death rate (untreated)</t>
+  </si>
+  <si>
+    <t>Death rate (on treatment)</t>
+  </si>
+  <si>
+    <t>Reinfection rate (recovered)</t>
+  </si>
+  <si>
+    <t>Latent treatment rate</t>
+  </si>
+  <si>
+    <t>Latent progression rate (treated)</t>
+  </si>
+  <si>
+    <t>Latent progression rate (untreated latent)</t>
+  </si>
+  <si>
+    <t>Recovery rate (latent)</t>
+  </si>
+  <si>
+    <t>Recovery rate (active)</t>
+  </si>
+  <si>
+    <t>Loss-to-followup (active)</t>
+  </si>
+  <si>
+    <t>Loss-to-followup (latent)</t>
+  </si>
+  <si>
+    <t>Active treatment rate</t>
+  </si>
+  <si>
+    <t>tmt_a</t>
+  </si>
+  <si>
+    <t>tmt_l</t>
+  </si>
+  <si>
+    <t>lu_prog</t>
+  </si>
+  <si>
+    <t>ltfu_l</t>
+  </si>
+  <si>
+    <t>lt_prog</t>
+  </si>
+  <si>
+    <t>rec_lat</t>
+  </si>
+  <si>
+    <t>rec_act</t>
+  </si>
+  <si>
+    <t>mort_t</t>
+  </si>
+  <si>
+    <t>mort_u</t>
+  </si>
+  <si>
+    <t>ltfu_a</t>
+  </si>
+  <si>
+    <t>reinf_rec</t>
+  </si>
+  <si>
+    <t>Population Size</t>
+  </si>
+  <si>
+    <t>test_act_prev</t>
+  </si>
+  <si>
+    <t>Population Sizes</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>sh_death</t>
+  </si>
+  <si>
+    <t>Mortality Rates</t>
+  </si>
+  <si>
+    <t>sh_cases</t>
   </si>
 </sst>
 </file>
@@ -248,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +358,26 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,12 +385,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,6 +415,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -344,12 +491,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -379,12 +526,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -588,88 +735,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -683,16 +849,16 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="5.77734375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="9" width="5.83203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -718,7 +884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -729,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -737,7 +903,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -748,7 +914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -762,7 +928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -773,7 +939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -787,7 +953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -795,7 +961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -808,61 +974,254 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="10">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="10">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8">
+        <v>200000</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -871,186 +1230,334 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="119.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="D11" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
       <c r="C12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
       <c r="C14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added column to cascade ('Characteristics' sheet --> column 'Plot Value'). If val == 'n' (case insensitive), then the plot is created when called in plotting.py This was in response to the probems encountered for full cascade with 13+ characteristics and 7 populations (which caused the UCL teams laptops to complain and refuse to create the plots without resetting the values for rcParams>defaultMax number of plots)
</commit_message>
<xml_diff>
--- a/data/cascade-simple.xlsx
+++ b/data/cascade-simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
   <si>
     <t>Code Label</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>sh_cases</t>
+  </si>
+  <si>
+    <t>Plot Value</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,6 +434,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -974,10 +989,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -987,13 +1002,14 @@
     <col min="3" max="3" width="11.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="14.6640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,20 +1025,23 @@
       <c r="E1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1036,19 +1055,20 @@
         <v>3</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="6"/>
+      <c r="K2" s="7"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1062,19 +1082,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1088,19 +1111,22 @@
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1116,21 +1142,24 @@
       <c r="E5" s="8">
         <v>10000</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1144,21 +1173,24 @@
         <v>2</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1172,27 +1204,30 @@
       <c r="E7" s="8">
         <v>200000</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="9"/>
+      <c r="J7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1202,26 +1237,29 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>